<commit_message>
Added L2 for PEMS, added emissions to L2 metrics for LEMS, modified PEMS subtract background to work for LEMS,
</commit_message>
<xml_diff>
--- a/Data/alcohol/alcohol_test1/alcohol_test1_TE_DataEntryForm.xlsx
+++ b/Data/alcohol/alcohol_test1/alcohol_test1_TE_DataEntryForm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\sam\LEMS-Data-Processing\Data\alcohol\alcohol_test1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden\Documents\GitHub\LEMS-Data-Processing\Data\alcohol\alcohol_test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1405,6 +1405,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1421,15 +1430,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1753,23 +1753,23 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.85546875" customWidth="1"/>
-    <col min="22" max="22" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.88671875" customWidth="1"/>
+    <col min="22" max="22" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44"/>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1791,18 +1791,18 @@
       <c r="S1" s="44"/>
       <c r="T1" s="44"/>
     </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44"/>
       <c r="B2" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
       <c r="H2" s="44"/>
       <c r="I2" s="81" t="s">
         <v>137</v>
@@ -1819,18 +1819,18 @@
       <c r="S2" s="44"/>
       <c r="T2" s="44"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44"/>
       <c r="B3" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="123">
+      <c r="C3" s="117">
         <v>1</v>
       </c>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
       <c r="H3" s="44"/>
       <c r="I3" s="84"/>
       <c r="J3" s="60"/>
@@ -1845,18 +1845,18 @@
       <c r="S3" s="44"/>
       <c r="T3" s="44"/>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="44"/>
       <c r="B4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="123" t="s">
+      <c r="C4" s="117" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
       <c r="H4" s="44"/>
       <c r="I4" s="84"/>
       <c r="J4" s="60"/>
@@ -1871,18 +1871,18 @@
       <c r="S4" s="44"/>
       <c r="T4" s="44"/>
     </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44"/>
       <c r="B5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="123" t="s">
+      <c r="C5" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
       <c r="H5" s="44"/>
       <c r="I5" s="62"/>
       <c r="J5" s="60"/>
@@ -1897,16 +1897,16 @@
       <c r="S5" s="44"/>
       <c r="T5" s="44"/>
     </row>
-    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="44"/>
       <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
       <c r="H6" s="44"/>
       <c r="I6" s="92" t="s">
         <v>138</v>
@@ -1923,18 +1923,18 @@
       <c r="S6" s="44"/>
       <c r="T6" s="44"/>
     </row>
-    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="123" t="s">
+      <c r="C7" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
       <c r="H7" s="44"/>
       <c r="I7" s="84"/>
       <c r="J7" s="60"/>
@@ -1949,7 +1949,7 @@
       <c r="S7" s="44"/>
       <c r="T7" s="44"/>
     </row>
-    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -1971,7 +1971,7 @@
       <c r="S8" s="44"/>
       <c r="T8" s="44"/>
     </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44"/>
       <c r="B9" s="45"/>
       <c r="C9" s="48" t="s">
@@ -1999,7 +1999,7 @@
       <c r="S9" s="44"/>
       <c r="T9" s="44"/>
     </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44"/>
       <c r="B10" s="15" t="s">
         <v>36</v>
@@ -2029,7 +2029,7 @@
       <c r="S10" s="44"/>
       <c r="T10" s="44"/>
     </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="44"/>
       <c r="B11" s="15" t="s">
         <v>37</v>
@@ -2059,7 +2059,7 @@
       <c r="S11" s="44"/>
       <c r="T11" s="44"/>
     </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="44"/>
       <c r="B12" s="15" t="s">
         <v>117</v>
@@ -2087,7 +2087,7 @@
       <c r="S12" s="44"/>
       <c r="T12" s="44"/>
     </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="44"/>
       <c r="B13" s="15" t="s">
         <v>133</v>
@@ -2115,7 +2115,7 @@
       <c r="S13" s="44"/>
       <c r="T13" s="44"/>
     </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
       <c r="B14" s="15" t="s">
         <v>38</v>
@@ -2145,7 +2145,7 @@
       <c r="S14" s="44"/>
       <c r="T14" s="44"/>
     </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44"/>
       <c r="B15" s="15" t="s">
         <v>118</v>
@@ -2173,7 +2173,7 @@
       <c r="S15" s="44"/>
       <c r="T15" s="44"/>
     </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="44"/>
       <c r="B16" s="20" t="s">
         <v>131</v>
@@ -2205,7 +2205,7 @@
       <c r="S16" s="44"/>
       <c r="T16" s="44"/>
     </row>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="20" t="s">
         <v>28</v>
@@ -2235,7 +2235,7 @@
       <c r="S17" s="44"/>
       <c r="T17" s="44"/>
     </row>
-    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
       <c r="B18" s="20" t="s">
         <v>29</v>
@@ -2263,7 +2263,7 @@
       <c r="S18" s="44"/>
       <c r="T18" s="44"/>
     </row>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="44"/>
       <c r="B19" s="20" t="s">
         <v>30</v>
@@ -2291,7 +2291,7 @@
       <c r="S19" s="44"/>
       <c r="T19" s="44"/>
     </row>
-    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="21" t="s">
         <v>31</v>
@@ -2319,7 +2319,7 @@
       <c r="S20" s="44"/>
       <c r="T20" s="44"/>
     </row>
-    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -2343,20 +2343,20 @@
       <c r="S21" s="44"/>
       <c r="T21" s="44"/>
     </row>
-    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="44"/>
       <c r="B22" s="23" t="s">
         <v>119</v>
       </c>
       <c r="C22" s="52"/>
-      <c r="D22" s="121" t="s">
+      <c r="D22" s="115" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="122"/>
-      <c r="F22" s="121" t="s">
+      <c r="E22" s="116"/>
+      <c r="F22" s="115" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="122"/>
+      <c r="G22" s="116"/>
       <c r="H22" s="44"/>
       <c r="I22" s="58"/>
       <c r="J22" s="79"/>
@@ -2371,7 +2371,7 @@
       <c r="S22" s="44"/>
       <c r="T22" s="44"/>
     </row>
-    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="47"/>
       <c r="C23" s="53" t="s">
@@ -2403,7 +2403,7 @@
       <c r="S23" s="44"/>
       <c r="T23" s="44"/>
     </row>
-    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="15" t="s">
         <v>124</v>
@@ -2435,7 +2435,7 @@
       <c r="S24" s="44"/>
       <c r="T24" s="44"/>
     </row>
-    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="44"/>
       <c r="B25" s="15" t="s">
         <v>125</v>
@@ -2467,7 +2467,7 @@
       <c r="S25" s="44"/>
       <c r="T25" s="44"/>
     </row>
-    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="15" t="s">
         <v>126</v>
@@ -2499,7 +2499,7 @@
       <c r="S26" s="44"/>
       <c r="T26" s="44"/>
     </row>
-    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="17" t="s">
         <v>127</v>
@@ -2529,7 +2529,7 @@
       <c r="S27" s="44"/>
       <c r="T27" s="44"/>
     </row>
-    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -2551,7 +2551,7 @@
       <c r="S28" s="44"/>
       <c r="T28" s="44"/>
     </row>
-    <row r="29" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="44"/>
       <c r="B29" s="24"/>
       <c r="C29" s="25"/>
@@ -2579,7 +2579,7 @@
       <c r="S29" s="44"/>
       <c r="T29" s="44"/>
     </row>
-    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="44"/>
       <c r="B30" s="31"/>
       <c r="C30" s="3"/>
@@ -2587,61 +2587,61 @@
         <v>3</v>
       </c>
       <c r="E30" s="16"/>
-      <c r="F30" s="115" t="s">
+      <c r="F30" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="116"/>
+      <c r="G30" s="119"/>
       <c r="H30" s="2"/>
       <c r="I30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J30" s="5"/>
-      <c r="K30" s="115" t="s">
+      <c r="K30" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="L30" s="116"/>
+      <c r="L30" s="119"/>
       <c r="M30" s="2"/>
       <c r="N30" s="16" t="s">
         <v>3</v>
       </c>
       <c r="O30" s="16"/>
-      <c r="P30" s="115" t="s">
+      <c r="P30" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="Q30" s="119"/>
+      <c r="Q30" s="122"/>
       <c r="R30" s="44"/>
       <c r="S30" s="44"/>
       <c r="T30" s="44"/>
     </row>
-    <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="44"/>
       <c r="B31" s="32"/>
       <c r="C31" s="3"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="117" t="s">
+      <c r="F31" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="118"/>
+      <c r="G31" s="121"/>
       <c r="H31" s="2"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="117" t="s">
+      <c r="K31" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="118"/>
+      <c r="L31" s="121"/>
       <c r="M31" s="2"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="117" t="s">
+      <c r="P31" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="Q31" s="120"/>
+      <c r="Q31" s="123"/>
       <c r="R31" s="44"/>
       <c r="S31" s="44"/>
       <c r="T31" s="44"/>
     </row>
-    <row r="32" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="44"/>
       <c r="B32" s="33" t="s">
         <v>6</v>
@@ -2691,7 +2691,7 @@
       <c r="S32" s="44"/>
       <c r="T32" s="44"/>
     </row>
-    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
       <c r="B33" s="34" t="s">
         <v>10</v>
@@ -2741,7 +2741,7 @@
       <c r="S33" s="44"/>
       <c r="T33" s="44"/>
     </row>
-    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="44"/>
       <c r="B34" s="34" t="s">
         <v>12</v>
@@ -2792,7 +2792,7 @@
       <c r="S34" s="44"/>
       <c r="T34" s="44"/>
     </row>
-    <row r="35" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="44"/>
       <c r="B35" s="34" t="s">
         <v>14</v>
@@ -2842,7 +2842,7 @@
       <c r="S35" s="44"/>
       <c r="T35" s="44"/>
     </row>
-    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="44"/>
       <c r="B36" s="37" t="s">
         <v>16</v>
@@ -2880,7 +2880,7 @@
       <c r="S36" s="44"/>
       <c r="T36" s="44"/>
     </row>
-    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="44"/>
       <c r="B37" s="37" t="s">
         <v>17</v>
@@ -2918,7 +2918,7 @@
       <c r="S37" s="44"/>
       <c r="T37" s="44"/>
     </row>
-    <row r="38" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="44"/>
       <c r="B38" s="37" t="s">
         <v>18</v>
@@ -2956,7 +2956,7 @@
       <c r="S38" s="44"/>
       <c r="T38" s="44"/>
     </row>
-    <row r="39" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="44"/>
       <c r="B39" s="34" t="s">
         <v>19</v>
@@ -3006,7 +3006,7 @@
       <c r="S39" s="44"/>
       <c r="T39" s="44"/>
     </row>
-    <row r="40" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="44"/>
       <c r="B40" s="37" t="s">
         <v>20</v>
@@ -3044,7 +3044,7 @@
       <c r="S40" s="44"/>
       <c r="T40" s="44"/>
     </row>
-    <row r="41" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="44"/>
       <c r="B41" s="37" t="s">
         <v>21</v>
@@ -3082,7 +3082,7 @@
       <c r="S41" s="44"/>
       <c r="T41" s="44"/>
     </row>
-    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="44"/>
       <c r="B42" s="37" t="s">
         <v>22</v>
@@ -3120,7 +3120,7 @@
       <c r="S42" s="44"/>
       <c r="T42" s="44"/>
     </row>
-    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44"/>
       <c r="B43" s="34" t="s">
         <v>25</v>
@@ -3158,7 +3158,7 @@
       <c r="S43" s="44"/>
       <c r="T43" s="44"/>
     </row>
-    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="44"/>
       <c r="B44" s="37" t="s">
         <v>23</v>
@@ -3190,7 +3190,7 @@
       <c r="S44" s="44"/>
       <c r="T44" s="44"/>
     </row>
-    <row r="45" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="44"/>
       <c r="B45" s="94" t="s">
         <v>26</v>
@@ -3222,7 +3222,7 @@
       <c r="S45" s="44"/>
       <c r="T45" s="44"/>
     </row>
-    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="44"/>
       <c r="B46" s="44"/>
       <c r="C46" s="44"/>
@@ -3244,7 +3244,7 @@
       <c r="S46" s="44"/>
       <c r="T46" s="44"/>
     </row>
-    <row r="47" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="44"/>
       <c r="B47" s="106" t="s">
         <v>156</v>
@@ -3268,7 +3268,7 @@
       <c r="S47" s="44"/>
       <c r="T47" s="44"/>
     </row>
-    <row r="48" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="44"/>
       <c r="B48" s="104"/>
       <c r="C48" s="112" t="s">
@@ -3296,7 +3296,7 @@
       <c r="S48" s="44"/>
       <c r="T48" s="44"/>
     </row>
-    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="44"/>
       <c r="B49" s="98" t="s">
         <v>157</v>
@@ -3324,7 +3324,7 @@
       <c r="S49" s="44"/>
       <c r="T49" s="44"/>
     </row>
-    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="44"/>
       <c r="B50" s="97" t="s">
         <v>158</v>
@@ -3352,7 +3352,7 @@
       <c r="S50" s="44"/>
       <c r="T50" s="44"/>
     </row>
-    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="44"/>
       <c r="B51" s="97" t="s">
         <v>159</v>
@@ -3380,7 +3380,7 @@
       <c r="S51" s="44"/>
       <c r="T51" s="44"/>
     </row>
-    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="44"/>
       <c r="B52" s="100" t="s">
         <v>160</v>
@@ -3409,7 +3409,7 @@
       <c r="S52" s="44"/>
       <c r="T52" s="44"/>
     </row>
-    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="44"/>
       <c r="B53" s="44"/>
       <c r="C53" s="44"/>
@@ -3431,7 +3431,7 @@
       <c r="S53" s="44"/>
       <c r="T53" s="44"/>
     </row>
-    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="44"/>
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
@@ -3453,7 +3453,7 @@
       <c r="S54" s="44"/>
       <c r="T54" s="44"/>
     </row>
-    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="44"/>
       <c r="B55" s="44"/>
       <c r="C55" s="44"/>
@@ -3475,7 +3475,7 @@
       <c r="S55" s="44"/>
       <c r="T55" s="44"/>
     </row>
-    <row r="56" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="44"/>
       <c r="B56" s="44"/>
       <c r="C56" s="44"/>
@@ -3497,7 +3497,7 @@
       <c r="S56" s="44"/>
       <c r="T56" s="44"/>
     </row>
-    <row r="57" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="44"/>
       <c r="B57" s="44"/>
       <c r="C57" s="44"/>
@@ -3519,7 +3519,7 @@
       <c r="S57" s="44"/>
       <c r="T57" s="44"/>
     </row>
-    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="44"/>
       <c r="B58" s="44"/>
       <c r="C58" s="44"/>
@@ -3541,7 +3541,7 @@
       <c r="S58" s="44"/>
       <c r="T58" s="44"/>
     </row>
-    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="44"/>
       <c r="B59" s="44"/>
       <c r="C59" s="44"/>
@@ -3563,7 +3563,7 @@
       <c r="S59" s="44"/>
       <c r="T59" s="44"/>
     </row>
-    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="44"/>
       <c r="B60" s="44"/>
       <c r="C60" s="44"/>
@@ -3585,7 +3585,7 @@
       <c r="S60" s="44"/>
       <c r="T60" s="44"/>
     </row>
-    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="44"/>
       <c r="B61" s="44"/>
       <c r="C61" s="44"/>
@@ -3607,7 +3607,7 @@
       <c r="S61" s="44"/>
       <c r="T61" s="44"/>
     </row>
-    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="44"/>
       <c r="B62" s="44"/>
       <c r="C62" s="44"/>
@@ -3629,7 +3629,7 @@
       <c r="S62" s="44"/>
       <c r="T62" s="44"/>
     </row>
-    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="44"/>
       <c r="B63" s="44"/>
       <c r="C63" s="44"/>
@@ -3651,7 +3651,7 @@
       <c r="S63" s="44"/>
       <c r="T63" s="44"/>
     </row>
-    <row r="64" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="44"/>
       <c r="B64" s="44"/>
       <c r="C64" s="44"/>
@@ -3673,7 +3673,7 @@
       <c r="S64" s="44"/>
       <c r="T64" s="44"/>
     </row>
-    <row r="65" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="44"/>
       <c r="B65" s="44"/>
       <c r="C65" s="44"/>
@@ -3695,7 +3695,7 @@
       <c r="S65" s="44"/>
       <c r="T65" s="44"/>
     </row>
-    <row r="66" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="44"/>
       <c r="B66" s="44"/>
       <c r="C66" s="44"/>
@@ -3717,7 +3717,7 @@
       <c r="S66" s="44"/>
       <c r="T66" s="44"/>
     </row>
-    <row r="67" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="44"/>
       <c r="B67" s="44"/>
       <c r="C67" s="44"/>
@@ -3739,7 +3739,7 @@
       <c r="S67" s="44"/>
       <c r="T67" s="44"/>
     </row>
-    <row r="68" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="44"/>
       <c r="B68" s="44"/>
       <c r="C68" s="44"/>
@@ -3761,7 +3761,7 @@
       <c r="S68" s="44"/>
       <c r="T68" s="44"/>
     </row>
-    <row r="69" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="44"/>
       <c r="B69" s="44"/>
       <c r="C69" s="44"/>
@@ -3783,7 +3783,7 @@
       <c r="S69" s="44"/>
       <c r="T69" s="44"/>
     </row>
-    <row r="70" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="44"/>
       <c r="B70" s="44"/>
       <c r="C70" s="44"/>
@@ -3805,7 +3805,7 @@
       <c r="S70" s="44"/>
       <c r="T70" s="44"/>
     </row>
-    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="44"/>
       <c r="B71" s="44"/>
       <c r="C71" s="44"/>
@@ -3827,7 +3827,7 @@
       <c r="S71" s="44"/>
       <c r="T71" s="44"/>
     </row>
-    <row r="72" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="44"/>
       <c r="B72" s="44"/>
       <c r="C72" s="44"/>
@@ -3849,7 +3849,7 @@
       <c r="S72" s="44"/>
       <c r="T72" s="44"/>
     </row>
-    <row r="73" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="44"/>
       <c r="B73" s="44"/>
       <c r="C73" s="44"/>
@@ -3871,7 +3871,7 @@
       <c r="S73" s="44"/>
       <c r="T73" s="44"/>
     </row>
-    <row r="74" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="44"/>
       <c r="B74" s="44"/>
       <c r="C74" s="44"/>
@@ -3893,7 +3893,7 @@
       <c r="S74" s="44"/>
       <c r="T74" s="44"/>
     </row>
-    <row r="75" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="44"/>
       <c r="B75" s="44"/>
       <c r="C75" s="44"/>
@@ -3915,7 +3915,7 @@
       <c r="S75" s="44"/>
       <c r="T75" s="44"/>
     </row>
-    <row r="76" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="44"/>
       <c r="B76" s="44"/>
       <c r="C76" s="44"/>
@@ -3937,7 +3937,7 @@
       <c r="S76" s="44"/>
       <c r="T76" s="44"/>
     </row>
-    <row r="77" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="44"/>
       <c r="B77" s="44"/>
       <c r="C77" s="44"/>
@@ -3959,7 +3959,7 @@
       <c r="S77" s="44"/>
       <c r="T77" s="44"/>
     </row>
-    <row r="78" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="44"/>
       <c r="B78" s="44"/>
       <c r="C78" s="44"/>
@@ -3981,7 +3981,7 @@
       <c r="S78" s="44"/>
       <c r="T78" s="44"/>
     </row>
-    <row r="79" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="44"/>
       <c r="B79" s="44"/>
       <c r="C79" s="44"/>
@@ -4003,7 +4003,7 @@
       <c r="S79" s="44"/>
       <c r="T79" s="44"/>
     </row>
-    <row r="80" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="44"/>
       <c r="B80" s="44"/>
       <c r="C80" s="44"/>
@@ -4025,7 +4025,7 @@
       <c r="S80" s="44"/>
       <c r="T80" s="44"/>
     </row>
-    <row r="81" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="44"/>
       <c r="B81" s="44"/>
       <c r="C81" s="44"/>
@@ -4047,7 +4047,7 @@
       <c r="S81" s="44"/>
       <c r="T81" s="44"/>
     </row>
-    <row r="82" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="44"/>
       <c r="B82" s="44"/>
       <c r="C82" s="44"/>
@@ -4069,7 +4069,7 @@
       <c r="S82" s="44"/>
       <c r="T82" s="44"/>
     </row>
-    <row r="83" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="44"/>
       <c r="B83" s="44"/>
       <c r="C83" s="44"/>
@@ -4091,7 +4091,7 @@
       <c r="S83" s="44"/>
       <c r="T83" s="44"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="44"/>
       <c r="B84" s="44"/>
       <c r="C84" s="44"/>
@@ -4113,7 +4113,7 @@
       <c r="S84" s="44"/>
       <c r="T84" s="44"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="44"/>
       <c r="E85" s="44"/>
       <c r="F85" s="44"/>
@@ -4132,7 +4132,7 @@
       <c r="S85" s="44"/>
       <c r="T85" s="44"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="44"/>
       <c r="E86" s="44"/>
       <c r="F86" s="44"/>
@@ -4153,6 +4153,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="P31:Q31"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="C2:G2"/>
@@ -4161,12 +4167,6 @@
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="P31:Q31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>